<commit_message>
version 2 finish project
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,7 +495,7 @@
         <v>101524</v>
       </c>
       <c r="H2" t="n">
-        <v>1.9283</v>
+        <v>1.92832</v>
       </c>
     </row>
     <row r="3">
@@ -523,7 +523,7 @@
         <v>104011</v>
       </c>
       <c r="H3" t="n">
-        <v>2.8551</v>
+        <v>2.85508</v>
       </c>
     </row>
     <row r="4">
@@ -551,7 +551,7 @@
         <v>104180</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5641</v>
+        <v>0.56411</v>
       </c>
     </row>
     <row r="5">
@@ -579,7 +579,7 @@
         <v>105007</v>
       </c>
       <c r="H5" t="n">
-        <v>1.1958</v>
+        <v>1.19581</v>
       </c>
     </row>
     <row r="6">
@@ -607,7 +607,7 @@
         <v>107435</v>
       </c>
       <c r="H6" t="n">
-        <v>2.7183</v>
+        <v>2.71832</v>
       </c>
     </row>
     <row r="7">
@@ -615,27 +615,27 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>XAU_TRY</t>
+          <t>EUR_TRY</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>1113</v>
+        <v>1378</v>
       </c>
       <c r="G7" t="n">
-        <v>108549</v>
+        <v>101378</v>
       </c>
       <c r="H7" t="n">
-        <v>1.4392</v>
+        <v>1.78212</v>
       </c>
     </row>
     <row r="8">
@@ -643,27 +643,27 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>EUR_TRY</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>6</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>XAU_TRY</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>28</v>
-      </c>
       <c r="E8" t="n">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
-        <v>1245</v>
+        <v>1143</v>
       </c>
       <c r="G8" t="n">
-        <v>109794</v>
+        <v>102521</v>
       </c>
       <c r="H8" t="n">
-        <v>1.5505</v>
+        <v>1.53061</v>
       </c>
     </row>
     <row r="9">
@@ -671,27 +671,27 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>XAU_TRY</t>
+          <t>EUR_TRY</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F9" t="n">
-        <v>199</v>
+        <v>248</v>
       </c>
       <c r="G9" t="n">
-        <v>109994</v>
+        <v>102770</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5826</v>
+        <v>0.64372</v>
       </c>
     </row>
     <row r="10">
@@ -699,7 +699,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -707,19 +707,19 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F10" t="n">
-        <v>1378</v>
+        <v>1449</v>
       </c>
       <c r="G10" t="n">
-        <v>101378</v>
+        <v>104219</v>
       </c>
       <c r="H10" t="n">
-        <v>1.7821</v>
+        <v>1.81362</v>
       </c>
     </row>
     <row r="11">
@@ -727,7 +727,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -735,19 +735,19 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F11" t="n">
-        <v>1143</v>
+        <v>3341</v>
       </c>
       <c r="G11" t="n">
-        <v>102521</v>
+        <v>107561</v>
       </c>
       <c r="H11" t="n">
-        <v>1.5306</v>
+        <v>3.61379</v>
       </c>
     </row>
     <row r="12">
@@ -755,27 +755,27 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>EUR_TRY</t>
+          <t>GBP_TRY</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
-        <v>248</v>
+        <v>4761</v>
       </c>
       <c r="G12" t="n">
-        <v>102770</v>
+        <v>104761</v>
       </c>
       <c r="H12" t="n">
-        <v>0.6437</v>
+        <v>5.17153</v>
       </c>
     </row>
     <row r="13">
@@ -783,27 +783,27 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>EUR_TRY</t>
+          <t>GBP_TRY</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
-        <v>1449</v>
+        <v>1774</v>
       </c>
       <c r="G13" t="n">
-        <v>104219</v>
+        <v>106535</v>
       </c>
       <c r="H13" t="n">
-        <v>1.8136</v>
+        <v>2.09807</v>
       </c>
     </row>
     <row r="14">
@@ -811,27 +811,27 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>EUR_TRY</t>
+          <t>GBP_TRY</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E14" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>4374</v>
+        <v>2967</v>
       </c>
       <c r="G14" t="n">
-        <v>108594</v>
+        <v>109503</v>
       </c>
       <c r="H14" t="n">
-        <v>4.6069</v>
+        <v>3.19174</v>
       </c>
     </row>
     <row r="15">
@@ -839,27 +839,27 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>EUR_TRY</t>
+          <t>GBP_TRY</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F15" t="n">
-        <v>1855</v>
+        <v>5749</v>
       </c>
       <c r="G15" t="n">
-        <v>110449</v>
+        <v>115252</v>
       </c>
       <c r="H15" t="n">
-        <v>2.1125</v>
+        <v>5.66171</v>
       </c>
     </row>
     <row r="16">
@@ -867,27 +867,27 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>EUR_TRY</t>
+          <t>USD_TRY</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
-        <v>100</v>
+        <v>6568</v>
       </c>
       <c r="G16" t="n">
-        <v>110549</v>
+        <v>106568</v>
       </c>
       <c r="H16" t="n">
-        <v>0.4922</v>
+        <v>6.98257</v>
       </c>
     </row>
     <row r="17">
@@ -895,27 +895,27 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>EUR_TRY</t>
+          <t>USD_TRY</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F17" t="n">
-        <v>161</v>
+        <v>2266</v>
       </c>
       <c r="G17" t="n">
-        <v>110710</v>
+        <v>108834</v>
       </c>
       <c r="H17" t="n">
-        <v>0.5467</v>
+        <v>2.53153</v>
       </c>
     </row>
     <row r="18">
@@ -923,335 +923,27 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>GBP_TRY</t>
+          <t>USD_TRY</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F18" t="n">
-        <v>4761</v>
+        <v>3076</v>
       </c>
       <c r="G18" t="n">
-        <v>104761</v>
+        <v>111910</v>
       </c>
       <c r="H18" t="n">
-        <v>5.1715</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>GBP_TRY</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>6</v>
-      </c>
-      <c r="E19" t="n">
-        <v>8</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1774</v>
-      </c>
-      <c r="G19" t="n">
-        <v>106535</v>
-      </c>
-      <c r="H19" t="n">
-        <v>2.0981</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>GBP_TRY</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>9</v>
-      </c>
-      <c r="E20" t="n">
-        <v>14</v>
-      </c>
-      <c r="F20" t="n">
-        <v>2967</v>
-      </c>
-      <c r="G20" t="n">
-        <v>109503</v>
-      </c>
-      <c r="H20" t="n">
-        <v>3.1917</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>3</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>GBP_TRY</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>15</v>
-      </c>
-      <c r="E21" t="n">
-        <v>20</v>
-      </c>
-      <c r="F21" t="n">
-        <v>5929</v>
-      </c>
-      <c r="G21" t="n">
-        <v>115432</v>
-      </c>
-      <c r="H21" t="n">
-        <v>5.8268</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>4</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>GBP_TRY</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>22</v>
-      </c>
-      <c r="E22" t="n">
-        <v>27</v>
-      </c>
-      <c r="F22" t="n">
-        <v>3818</v>
-      </c>
-      <c r="G22" t="n">
-        <v>119251</v>
-      </c>
-      <c r="H22" t="n">
-        <v>3.7158</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>5</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>GBP_TRY</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>28</v>
-      </c>
-      <c r="E23" t="n">
-        <v>29</v>
-      </c>
-      <c r="F23" t="n">
-        <v>96</v>
-      </c>
-      <c r="G23" t="n">
-        <v>119347</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.4815</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>USD_TRY</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" t="n">
-        <v>9</v>
-      </c>
-      <c r="F24" t="n">
-        <v>6568</v>
-      </c>
-      <c r="G24" t="n">
-        <v>106568</v>
-      </c>
-      <c r="H24" t="n">
-        <v>6.9826</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>USD_TRY</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>10</v>
-      </c>
-      <c r="E25" t="n">
-        <v>14</v>
-      </c>
-      <c r="F25" t="n">
-        <v>2266</v>
-      </c>
-      <c r="G25" t="n">
-        <v>108834</v>
-      </c>
-      <c r="H25" t="n">
-        <v>2.5315</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>2</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>USD_TRY</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>16</v>
-      </c>
-      <c r="E26" t="n">
-        <v>20</v>
-      </c>
-      <c r="F26" t="n">
-        <v>3206</v>
-      </c>
-      <c r="G26" t="n">
-        <v>112041</v>
-      </c>
-      <c r="H26" t="n">
-        <v>3.3531</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>3</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>USD_TRY</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>22</v>
-      </c>
-      <c r="E27" t="n">
-        <v>24</v>
-      </c>
-      <c r="F27" t="n">
-        <v>2741</v>
-      </c>
-      <c r="G27" t="n">
-        <v>114782</v>
-      </c>
-      <c r="H27" t="n">
-        <v>2.8523</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="n">
-        <v>4</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>USD_TRY</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>25</v>
-      </c>
-      <c r="E28" t="n">
-        <v>27</v>
-      </c>
-      <c r="F28" t="n">
-        <v>1637</v>
-      </c>
-      <c r="G28" t="n">
-        <v>116420</v>
-      </c>
-      <c r="H28" t="n">
-        <v>1.8306</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="n">
-        <v>5</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>USD_TRY</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>29</v>
-      </c>
-      <c r="E29" t="n">
-        <v>30</v>
-      </c>
-      <c r="F29" t="n">
-        <v>405</v>
-      </c>
-      <c r="G29" t="n">
-        <v>116826</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0.75</v>
+        <v>3.23281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>